<commit_message>
Tempo de Execução adicionado
</commit_message>
<xml_diff>
--- a/trabalho-final/files/agendaDeHorarios.xlsx
+++ b/trabalho-final/files/agendaDeHorarios.xlsx
@@ -7,10 +7,10 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Todos" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Perdoes" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Lavras" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Perdoes" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Bambui" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Bambui" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Todos" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -528,29 +528,13 @@
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>68 : 52 anos, Perdoes | 99 : 25 anos, Lavras | 94 : 35 anos, Medeiros | 74 : 18 anos, Perdoes</t>
-        </is>
-      </c>
-      <c r="C2" s="3" t="inlineStr">
-        <is>
-          <t>16 : 20 anos, Bambui | 57 : 52 anos, Bambui | 76 : 28 anos, Bom Sucesso</t>
-        </is>
-      </c>
-      <c r="D2" s="4" t="inlineStr">
-        <is>
-          <t>21 : 62 anos, Bambui</t>
-        </is>
-      </c>
-      <c r="E2" s="4" t="inlineStr">
-        <is>
-          <t>19 : 24 anos, Guarulhos | 65 : 50 anos, Lavras</t>
-        </is>
-      </c>
-      <c r="F2" s="4" t="inlineStr">
-        <is>
-          <t>69 : 32 anos, Lavras</t>
-        </is>
-      </c>
+          <t>68 : 52 anos, Perdoes</t>
+        </is>
+      </c>
+      <c r="C2" s="5" t="inlineStr"/>
+      <c r="D2" s="5" t="inlineStr"/>
+      <c r="E2" s="5" t="inlineStr"/>
+      <c r="F2" s="5" t="inlineStr"/>
       <c r="G2" s="3" t="inlineStr">
         <is>
           <t>52 : 22 anos, Perdoes | 62 : 50 anos, Perdoes | 79 : 17 anos, Perdoes</t>
@@ -563,36 +547,12 @@
           <t>09:00</t>
         </is>
       </c>
-      <c r="B3" s="3" t="inlineStr">
-        <is>
-          <t>58 : 22 anos, Lavras | 70 : 21 anos, Ijaci</t>
-        </is>
-      </c>
-      <c r="C3" s="3" t="inlineStr">
-        <is>
-          <t>53 : 21 anos, Ilheus</t>
-        </is>
-      </c>
-      <c r="D3" s="3" t="inlineStr">
-        <is>
-          <t>7 : 24 anos, Bambui</t>
-        </is>
-      </c>
-      <c r="E3" s="3" t="inlineStr">
-        <is>
-          <t>61 : 22 anos, Lavras</t>
-        </is>
-      </c>
-      <c r="F3" s="4" t="inlineStr">
-        <is>
-          <t>36 : 71 anos, Guarapari</t>
-        </is>
-      </c>
-      <c r="G3" s="3" t="inlineStr">
-        <is>
-          <t>60 : 21 anos, Lavras</t>
-        </is>
-      </c>
+      <c r="B3" s="5" t="inlineStr"/>
+      <c r="C3" s="5" t="inlineStr"/>
+      <c r="D3" s="5" t="inlineStr"/>
+      <c r="E3" s="5" t="inlineStr"/>
+      <c r="F3" s="5" t="inlineStr"/>
+      <c r="G3" s="5" t="inlineStr"/>
     </row>
     <row r="4" ht="40" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
@@ -600,32 +560,12 @@
           <t>10:00</t>
         </is>
       </c>
-      <c r="B4" s="3" t="inlineStr">
-        <is>
-          <t>41 : 21 anos, Ijaci | 82 : 21 anos, Vicosa</t>
-        </is>
-      </c>
+      <c r="B4" s="5" t="inlineStr"/>
       <c r="C4" s="5" t="inlineStr"/>
-      <c r="D4" s="4" t="inlineStr">
-        <is>
-          <t>26 : 20 anos, Lavras</t>
-        </is>
-      </c>
-      <c r="E4" s="3" t="inlineStr">
-        <is>
-          <t>6 : 23 anos, Lavras | 12 : 27 anos, Uberaba</t>
-        </is>
-      </c>
-      <c r="F4" s="3" t="inlineStr">
-        <is>
-          <t>24 : 19 anos, Arcos | 71 : 45 anos, Medeiros</t>
-        </is>
-      </c>
-      <c r="G4" s="3" t="inlineStr">
-        <is>
-          <t>81 : 23 anos, Sao Paulo</t>
-        </is>
-      </c>
+      <c r="D4" s="5" t="inlineStr"/>
+      <c r="E4" s="5" t="inlineStr"/>
+      <c r="F4" s="5" t="inlineStr"/>
+      <c r="G4" s="5" t="inlineStr"/>
     </row>
     <row r="5" ht="40" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
@@ -633,32 +573,12 @@
           <t>11:00</t>
         </is>
       </c>
-      <c r="B5" s="3" t="inlineStr">
-        <is>
-          <t>37 : 19 anos, Lavras</t>
-        </is>
-      </c>
-      <c r="C5" s="3" t="inlineStr">
-        <is>
-          <t>2 : 21 anos, Lavras</t>
-        </is>
-      </c>
-      <c r="D5" s="3" t="inlineStr">
-        <is>
-          <t>17 : 19 anos, Sao Paulo</t>
-        </is>
-      </c>
+      <c r="B5" s="5" t="inlineStr"/>
+      <c r="C5" s="5" t="inlineStr"/>
+      <c r="D5" s="5" t="inlineStr"/>
       <c r="E5" s="5" t="inlineStr"/>
-      <c r="F5" s="3" t="inlineStr">
-        <is>
-          <t>51 : 26 anos, Macuco de Minas</t>
-        </is>
-      </c>
-      <c r="G5" s="3" t="inlineStr">
-        <is>
-          <t>86 : 22 anos, Oliveira</t>
-        </is>
-      </c>
+      <c r="F5" s="5" t="inlineStr"/>
+      <c r="G5" s="5" t="inlineStr"/>
     </row>
     <row r="6" ht="40" customHeight="1">
       <c r="A6" s="2" t="inlineStr">
@@ -668,11 +588,7 @@
       </c>
       <c r="B6" s="5" t="inlineStr"/>
       <c r="C6" s="5" t="inlineStr"/>
-      <c r="D6" s="3" t="inlineStr">
-        <is>
-          <t>45 : 22 anos, Campo Belo</t>
-        </is>
-      </c>
+      <c r="D6" s="5" t="inlineStr"/>
       <c r="E6" s="5" t="inlineStr"/>
       <c r="F6" s="5" t="inlineStr"/>
       <c r="G6" s="5" t="inlineStr"/>
@@ -683,22 +599,14 @@
           <t>13:00</t>
         </is>
       </c>
-      <c r="B7" s="3" t="inlineStr">
-        <is>
-          <t>14 : 21 anos, Japaraiba | 88 : 21 anos, Bambui</t>
-        </is>
-      </c>
+      <c r="B7" s="5" t="inlineStr"/>
       <c r="C7" s="5" t="inlineStr"/>
       <c r="D7" s="5" t="inlineStr"/>
-      <c r="E7" s="3" t="inlineStr">
-        <is>
-          <t>20 : 52 anos, Bambui</t>
-        </is>
-      </c>
+      <c r="E7" s="5" t="inlineStr"/>
       <c r="F7" s="5" t="inlineStr"/>
       <c r="G7" s="3" t="inlineStr">
         <is>
-          <t>40 : 23 anos, Perdoes | 75 : 31 anos, Lavras</t>
+          <t>40 : 23 anos, Perdoes</t>
         </is>
       </c>
     </row>
@@ -708,36 +616,12 @@
           <t>14:00</t>
         </is>
       </c>
-      <c r="B8" s="3" t="inlineStr">
-        <is>
-          <t>46 : 21 anos, Jundiai</t>
-        </is>
-      </c>
-      <c r="C8" s="3" t="inlineStr">
-        <is>
-          <t>44 : 21 anos, Varginha | 89 : 22 anos, Divinopolis | 97 : 54 anos, Bambui</t>
-        </is>
-      </c>
-      <c r="D8" s="3" t="inlineStr">
-        <is>
-          <t>27 : 49 anos, Bambui</t>
-        </is>
-      </c>
-      <c r="E8" s="3" t="inlineStr">
-        <is>
-          <t>5 : 33 anos, Bambui</t>
-        </is>
-      </c>
-      <c r="F8" s="3" t="inlineStr">
-        <is>
-          <t>25 : 21 anos, Bambui</t>
-        </is>
-      </c>
-      <c r="G8" s="3" t="inlineStr">
-        <is>
-          <t>8 : 21 anos, Osasco</t>
-        </is>
-      </c>
+      <c r="B8" s="5" t="inlineStr"/>
+      <c r="C8" s="5" t="inlineStr"/>
+      <c r="D8" s="5" t="inlineStr"/>
+      <c r="E8" s="5" t="inlineStr"/>
+      <c r="F8" s="5" t="inlineStr"/>
+      <c r="G8" s="5" t="inlineStr"/>
     </row>
     <row r="9" ht="40" customHeight="1">
       <c r="A9" s="2" t="inlineStr">
@@ -745,32 +629,12 @@
           <t>15:00</t>
         </is>
       </c>
-      <c r="B9" s="3" t="inlineStr">
-        <is>
-          <t>38 : 19 anos, Bambui | 66 : 15 anos, Lavras</t>
-        </is>
-      </c>
-      <c r="C9" s="3" t="inlineStr">
-        <is>
-          <t>34 : 19 anos, Sorocaba | 83 : 20 anos, Lagoa da Prata</t>
-        </is>
-      </c>
-      <c r="D9" s="3" t="inlineStr">
-        <is>
-          <t>31 : 35 anos, Bambui | 39 : 23 anos, Sao Joao Del Rei | 48 : 22 anos, Varginha</t>
-        </is>
-      </c>
-      <c r="E9" s="3" t="inlineStr">
-        <is>
-          <t>9 : 29 anos, Araraquara | 18 : 49 anos, Bambui | 80 : 32 anos, Belo Horizonte</t>
-        </is>
-      </c>
+      <c r="B9" s="5" t="inlineStr"/>
+      <c r="C9" s="5" t="inlineStr"/>
+      <c r="D9" s="5" t="inlineStr"/>
+      <c r="E9" s="5" t="inlineStr"/>
       <c r="F9" s="5" t="inlineStr"/>
-      <c r="G9" s="3" t="inlineStr">
-        <is>
-          <t>4 : 20 anos, Guarulhos | 73 : 23 anos, Uba</t>
-        </is>
-      </c>
+      <c r="G9" s="5" t="inlineStr"/>
     </row>
     <row r="10" ht="40" customHeight="1">
       <c r="A10" s="2" t="inlineStr">
@@ -778,32 +642,12 @@
           <t>16:00</t>
         </is>
       </c>
-      <c r="B10" s="3" t="inlineStr">
-        <is>
-          <t>84 : 19 anos, Sorocaba</t>
-        </is>
-      </c>
-      <c r="C10" s="3" t="inlineStr">
-        <is>
-          <t>32 : 21 anos, Guarapari | 64 : 21 anos, Oliveira</t>
-        </is>
-      </c>
-      <c r="D10" s="3" t="inlineStr">
-        <is>
-          <t>1 : 20 anos, Bambui | 29 : 20 anos, Pocos de Caldas | 30 : 20 anos, Lagoa da Prata | 33 : 21 anos, Lavras | 85 : 19 anos, Bambui</t>
-        </is>
-      </c>
+      <c r="B10" s="5" t="inlineStr"/>
+      <c r="C10" s="5" t="inlineStr"/>
+      <c r="D10" s="5" t="inlineStr"/>
       <c r="E10" s="5" t="inlineStr"/>
-      <c r="F10" s="4" t="inlineStr">
-        <is>
-          <t>91 : 37 anos, Lavras</t>
-        </is>
-      </c>
-      <c r="G10" s="3" t="inlineStr">
-        <is>
-          <t>54 : 29 anos, Lavras</t>
-        </is>
-      </c>
+      <c r="F10" s="5" t="inlineStr"/>
+      <c r="G10" s="5" t="inlineStr"/>
     </row>
     <row r="11" ht="40" customHeight="1">
       <c r="A11" s="2" t="inlineStr">
@@ -812,29 +656,21 @@
         </is>
       </c>
       <c r="B11" s="5" t="inlineStr"/>
-      <c r="C11" s="4" t="inlineStr">
-        <is>
-          <t>13 : 23 anos, Uberlandia | 22 : 60 anos, Bambui</t>
-        </is>
-      </c>
+      <c r="C11" s="5" t="inlineStr"/>
       <c r="D11" s="3" t="inlineStr">
         <is>
-          <t>11 : 20 anos, Medeiros | 42 : 21 anos, Bambui | 50 : 19 anos, Perdoes | 59 : 21 anos, Bambui | 67 : 20 anos, Bambui</t>
-        </is>
-      </c>
-      <c r="E11" s="3" t="inlineStr">
-        <is>
-          <t>35 : 42 anos, Colatina | 100 : 23 anos, Ijaci</t>
-        </is>
-      </c>
+          <t>50 : 19 anos, Perdoes | 74 : 18 anos, Perdoes</t>
+        </is>
+      </c>
+      <c r="E11" s="5" t="inlineStr"/>
       <c r="F11" s="3" t="inlineStr">
         <is>
-          <t>55 : 16 anos, Perdoes | 78 : 21 anos, Espinosa | 87 : 23 anos, Itajuba</t>
+          <t>55 : 16 anos, Perdoes</t>
         </is>
       </c>
       <c r="G11" s="3" t="inlineStr">
         <is>
-          <t>63 : 20 anos, Perdoes | 95 : 24 anos, Itajuba | 101 : 20 anos, Arcos</t>
+          <t>63 : 20 anos, Perdoes</t>
         </is>
       </c>
     </row>
@@ -846,39 +682,27 @@
       </c>
       <c r="B12" s="3" t="inlineStr">
         <is>
-          <t>43 : 24 anos, Perdoes | 47 : 21 anos, Campo Belo | 72 : 32 anos, Lavras</t>
-        </is>
-      </c>
-      <c r="C12" s="3" t="inlineStr">
-        <is>
-          <t>90 : 21 anos, Lavras | 92 : 20 anos, Areado</t>
-        </is>
-      </c>
+          <t>43 : 24 anos, Perdoes</t>
+        </is>
+      </c>
+      <c r="C12" s="5" t="inlineStr"/>
       <c r="D12" s="3" t="inlineStr">
         <is>
-          <t>23 : 16 anos, Guarulhos | 28 : 21 anos, Oliveira | 49 : 23 anos, Perdoes | 98 : 22 anos, Perdoes</t>
-        </is>
-      </c>
-      <c r="E12" s="3" t="inlineStr">
-        <is>
-          <t>3 : 22 anos, Lavras</t>
-        </is>
-      </c>
+          <t>49 : 23 anos, Perdoes</t>
+        </is>
+      </c>
+      <c r="E12" s="5" t="inlineStr"/>
       <c r="F12" s="3" t="inlineStr">
         <is>
-          <t>56 : 19 anos, Perdoes | 77 : 23 anos, Lavras</t>
-        </is>
-      </c>
-      <c r="G12" s="3" t="inlineStr">
-        <is>
-          <t>15 : 20 anos, Lagoa da Prata | 96 : 21 anos, Lavras</t>
-        </is>
-      </c>
+          <t>56 : 19 anos, Perdoes | 98 : 22 anos, Perdoes</t>
+        </is>
+      </c>
+      <c r="G12" s="5" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="G13" s="6" t="inlineStr">
         <is>
-          <t>Horários ocupados: 53/66</t>
+          <t>Horários ocupados: 9/66</t>
         </is>
       </c>
     </row>
@@ -947,25 +771,21 @@
           <t>08:00</t>
         </is>
       </c>
-      <c r="B2" s="3" t="inlineStr">
+      <c r="B2" s="4" t="inlineStr">
+        <is>
+          <t>69 : 32 anos, Lavras</t>
+        </is>
+      </c>
+      <c r="C2" s="5" t="inlineStr"/>
+      <c r="D2" s="5" t="inlineStr"/>
+      <c r="E2" s="4" t="inlineStr">
+        <is>
+          <t>65 : 50 anos, Lavras</t>
+        </is>
+      </c>
+      <c r="F2" s="3" t="inlineStr">
         <is>
           <t>61 : 22 anos, Lavras</t>
-        </is>
-      </c>
-      <c r="C2" s="5" t="inlineStr"/>
-      <c r="D2" s="3" t="inlineStr">
-        <is>
-          <t>6 : 23 anos, Lavras</t>
-        </is>
-      </c>
-      <c r="E2" s="4" t="inlineStr">
-        <is>
-          <t>65 : 50 anos, Lavras</t>
-        </is>
-      </c>
-      <c r="F2" s="3" t="inlineStr">
-        <is>
-          <t>99 : 25 anos, Lavras</t>
         </is>
       </c>
       <c r="G2" s="5" t="inlineStr"/>
@@ -978,15 +798,11 @@
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>58 : 22 anos, Lavras</t>
+          <t>58 : 22 anos, Lavras | 90 : 21 anos, Lavras</t>
         </is>
       </c>
       <c r="C3" s="5" t="inlineStr"/>
-      <c r="D3" s="3" t="inlineStr">
-        <is>
-          <t>90 : 21 anos, Lavras</t>
-        </is>
-      </c>
+      <c r="D3" s="5" t="inlineStr"/>
       <c r="E3" s="5" t="inlineStr"/>
       <c r="F3" s="5" t="inlineStr"/>
       <c r="G3" s="3" t="inlineStr">
@@ -1007,13 +823,17 @@
         </is>
       </c>
       <c r="C4" s="5" t="inlineStr"/>
-      <c r="D4" s="4" t="inlineStr">
+      <c r="D4" s="3" t="inlineStr">
+        <is>
+          <t>6 : 23 anos, Lavras</t>
+        </is>
+      </c>
+      <c r="E4" s="5" t="inlineStr"/>
+      <c r="F4" s="4" t="inlineStr">
         <is>
           <t>26 : 20 anos, Lavras</t>
         </is>
       </c>
-      <c r="E4" s="5" t="inlineStr"/>
-      <c r="F4" s="5" t="inlineStr"/>
       <c r="G4" s="5" t="inlineStr"/>
     </row>
     <row r="5" ht="40" customHeight="1">
@@ -1023,18 +843,14 @@
         </is>
       </c>
       <c r="B5" s="5" t="inlineStr"/>
-      <c r="C5" s="5" t="inlineStr"/>
-      <c r="D5" s="3" t="inlineStr">
+      <c r="C5" s="3" t="inlineStr">
         <is>
           <t>2 : 21 anos, Lavras</t>
         </is>
       </c>
+      <c r="D5" s="5" t="inlineStr"/>
       <c r="E5" s="5" t="inlineStr"/>
-      <c r="F5" s="4" t="inlineStr">
-        <is>
-          <t>69 : 32 anos, Lavras</t>
-        </is>
-      </c>
+      <c r="F5" s="5" t="inlineStr"/>
       <c r="G5" s="5" t="inlineStr"/>
     </row>
     <row r="6" ht="40" customHeight="1">
@@ -1047,7 +863,11 @@
       <c r="C6" s="5" t="inlineStr"/>
       <c r="D6" s="5" t="inlineStr"/>
       <c r="E6" s="5" t="inlineStr"/>
-      <c r="F6" s="5" t="inlineStr"/>
+      <c r="F6" s="3" t="inlineStr">
+        <is>
+          <t>99 : 25 anos, Lavras</t>
+        </is>
+      </c>
       <c r="G6" s="5" t="inlineStr"/>
     </row>
     <row r="7" ht="40" customHeight="1">
@@ -1060,12 +880,12 @@
       <c r="C7" s="5" t="inlineStr"/>
       <c r="D7" s="5" t="inlineStr"/>
       <c r="E7" s="5" t="inlineStr"/>
-      <c r="F7" s="5" t="inlineStr"/>
-      <c r="G7" s="3" t="inlineStr">
+      <c r="F7" s="3" t="inlineStr">
         <is>
           <t>75 : 31 anos, Lavras</t>
         </is>
       </c>
+      <c r="G7" s="5" t="inlineStr"/>
     </row>
     <row r="8" ht="40" customHeight="1">
       <c r="A8" s="2" t="inlineStr">
@@ -1092,7 +912,11 @@
         </is>
       </c>
       <c r="C9" s="5" t="inlineStr"/>
-      <c r="D9" s="5" t="inlineStr"/>
+      <c r="D9" s="3" t="inlineStr">
+        <is>
+          <t>33 : 21 anos, Lavras</t>
+        </is>
+      </c>
       <c r="E9" s="5" t="inlineStr"/>
       <c r="F9" s="5" t="inlineStr"/>
       <c r="G9" s="5" t="inlineStr"/>
@@ -1105,11 +929,7 @@
       </c>
       <c r="B10" s="5" t="inlineStr"/>
       <c r="C10" s="5" t="inlineStr"/>
-      <c r="D10" s="3" t="inlineStr">
-        <is>
-          <t>33 : 21 anos, Lavras</t>
-        </is>
-      </c>
+      <c r="D10" s="5" t="inlineStr"/>
       <c r="E10" s="5" t="inlineStr"/>
       <c r="F10" s="4" t="inlineStr">
         <is>
@@ -1141,18 +961,22 @@
           <t>18:00</t>
         </is>
       </c>
-      <c r="B12" s="5" t="inlineStr"/>
+      <c r="B12" s="3" t="inlineStr">
+        <is>
+          <t>72 : 32 anos, Lavras</t>
+        </is>
+      </c>
       <c r="C12" s="5" t="inlineStr"/>
-      <c r="D12" s="3" t="inlineStr">
-        <is>
-          <t>72 : 32 anos, Lavras</t>
-        </is>
-      </c>
-      <c r="E12" s="5" t="inlineStr"/>
+      <c r="D12" s="5" t="inlineStr"/>
+      <c r="E12" s="3" t="inlineStr">
+        <is>
+          <t>3 : 22 anos, Lavras</t>
+        </is>
+      </c>
       <c r="F12" s="5" t="inlineStr"/>
       <c r="G12" s="3" t="inlineStr">
         <is>
-          <t>3 : 22 anos, Lavras | 77 : 23 anos, Lavras | 96 : 21 anos, Lavras</t>
+          <t>77 : 23 anos, Lavras | 96 : 21 anos, Lavras</t>
         </is>
       </c>
     </row>
@@ -1228,20 +1052,20 @@
           <t>08:00</t>
         </is>
       </c>
-      <c r="B2" s="3" t="inlineStr">
-        <is>
-          <t>68 : 52 anos, Perdoes</t>
-        </is>
-      </c>
-      <c r="C2" s="5" t="inlineStr"/>
-      <c r="D2" s="5" t="inlineStr"/>
+      <c r="B2" s="5" t="inlineStr"/>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>57 : 52 anos, Bambui</t>
+        </is>
+      </c>
+      <c r="D2" s="4" t="inlineStr">
+        <is>
+          <t>21 : 62 anos, Bambui</t>
+        </is>
+      </c>
       <c r="E2" s="5" t="inlineStr"/>
       <c r="F2" s="5" t="inlineStr"/>
-      <c r="G2" s="3" t="inlineStr">
-        <is>
-          <t>52 : 22 anos, Perdoes | 62 : 50 anos, Perdoes | 79 : 17 anos, Perdoes</t>
-        </is>
-      </c>
+      <c r="G2" s="5" t="inlineStr"/>
     </row>
     <row r="3" ht="40" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
@@ -1251,7 +1075,11 @@
       </c>
       <c r="B3" s="5" t="inlineStr"/>
       <c r="C3" s="5" t="inlineStr"/>
-      <c r="D3" s="5" t="inlineStr"/>
+      <c r="D3" s="3" t="inlineStr">
+        <is>
+          <t>7 : 24 anos, Bambui | 59 : 21 anos, Bambui</t>
+        </is>
+      </c>
       <c r="E3" s="5" t="inlineStr"/>
       <c r="F3" s="5" t="inlineStr"/>
       <c r="G3" s="5" t="inlineStr"/>
@@ -1301,16 +1129,16 @@
           <t>13:00</t>
         </is>
       </c>
-      <c r="B7" s="5" t="inlineStr"/>
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>20 : 52 anos, Bambui | 42 : 21 anos, Bambui</t>
+        </is>
+      </c>
       <c r="C7" s="5" t="inlineStr"/>
       <c r="D7" s="5" t="inlineStr"/>
       <c r="E7" s="5" t="inlineStr"/>
       <c r="F7" s="5" t="inlineStr"/>
-      <c r="G7" s="3" t="inlineStr">
-        <is>
-          <t>40 : 23 anos, Perdoes</t>
-        </is>
-      </c>
+      <c r="G7" s="5" t="inlineStr"/>
     </row>
     <row r="8" ht="40" customHeight="1">
       <c r="A8" s="2" t="inlineStr">
@@ -1320,9 +1148,21 @@
       </c>
       <c r="B8" s="5" t="inlineStr"/>
       <c r="C8" s="5" t="inlineStr"/>
-      <c r="D8" s="5" t="inlineStr"/>
-      <c r="E8" s="5" t="inlineStr"/>
-      <c r="F8" s="5" t="inlineStr"/>
+      <c r="D8" s="3" t="inlineStr">
+        <is>
+          <t>25 : 21 anos, Bambui</t>
+        </is>
+      </c>
+      <c r="E8" s="3" t="inlineStr">
+        <is>
+          <t>5 : 33 anos, Bambui</t>
+        </is>
+      </c>
+      <c r="F8" s="3" t="inlineStr">
+        <is>
+          <t>27 : 49 anos, Bambui</t>
+        </is>
+      </c>
       <c r="G8" s="5" t="inlineStr"/>
     </row>
     <row r="9" ht="40" customHeight="1">
@@ -1331,11 +1171,27 @@
           <t>15:00</t>
         </is>
       </c>
-      <c r="B9" s="5" t="inlineStr"/>
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t>38 : 19 anos, Bambui | 88 : 21 anos, Bambui</t>
+        </is>
+      </c>
       <c r="C9" s="5" t="inlineStr"/>
-      <c r="D9" s="5" t="inlineStr"/>
-      <c r="E9" s="5" t="inlineStr"/>
-      <c r="F9" s="5" t="inlineStr"/>
+      <c r="D9" s="3" t="inlineStr">
+        <is>
+          <t>31 : 35 anos, Bambui | 97 : 54 anos, Bambui</t>
+        </is>
+      </c>
+      <c r="E9" s="3" t="inlineStr">
+        <is>
+          <t>18 : 49 anos, Bambui</t>
+        </is>
+      </c>
+      <c r="F9" s="3" t="inlineStr">
+        <is>
+          <t>16 : 20 anos, Bambui</t>
+        </is>
+      </c>
       <c r="G9" s="5" t="inlineStr"/>
     </row>
     <row r="10" ht="40" customHeight="1">
@@ -1346,8 +1202,16 @@
       </c>
       <c r="B10" s="5" t="inlineStr"/>
       <c r="C10" s="5" t="inlineStr"/>
-      <c r="D10" s="5" t="inlineStr"/>
-      <c r="E10" s="5" t="inlineStr"/>
+      <c r="D10" s="3" t="inlineStr">
+        <is>
+          <t>67 : 20 anos, Bambui | 85 : 19 anos, Bambui</t>
+        </is>
+      </c>
+      <c r="E10" s="3" t="inlineStr">
+        <is>
+          <t>1 : 20 anos, Bambui</t>
+        </is>
+      </c>
       <c r="F10" s="5" t="inlineStr"/>
       <c r="G10" s="5" t="inlineStr"/>
     </row>
@@ -1359,22 +1223,14 @@
       </c>
       <c r="B11" s="5" t="inlineStr"/>
       <c r="C11" s="5" t="inlineStr"/>
-      <c r="D11" s="3" t="inlineStr">
-        <is>
-          <t>50 : 19 anos, Perdoes | 74 : 18 anos, Perdoes</t>
+      <c r="D11" s="4" t="inlineStr">
+        <is>
+          <t>22 : 60 anos, Bambui</t>
         </is>
       </c>
       <c r="E11" s="5" t="inlineStr"/>
-      <c r="F11" s="3" t="inlineStr">
-        <is>
-          <t>55 : 16 anos, Perdoes</t>
-        </is>
-      </c>
-      <c r="G11" s="3" t="inlineStr">
-        <is>
-          <t>63 : 20 anos, Perdoes</t>
-        </is>
-      </c>
+      <c r="F11" s="5" t="inlineStr"/>
+      <c r="G11" s="5" t="inlineStr"/>
     </row>
     <row r="12" ht="40" customHeight="1">
       <c r="A12" s="2" t="inlineStr">
@@ -1382,29 +1238,17 @@
           <t>18:00</t>
         </is>
       </c>
-      <c r="B12" s="3" t="inlineStr">
-        <is>
-          <t>43 : 24 anos, Perdoes</t>
-        </is>
-      </c>
+      <c r="B12" s="5" t="inlineStr"/>
       <c r="C12" s="5" t="inlineStr"/>
-      <c r="D12" s="3" t="inlineStr">
-        <is>
-          <t>49 : 23 anos, Perdoes</t>
-        </is>
-      </c>
+      <c r="D12" s="5" t="inlineStr"/>
       <c r="E12" s="5" t="inlineStr"/>
-      <c r="F12" s="3" t="inlineStr">
-        <is>
-          <t>56 : 19 anos, Perdoes | 98 : 22 anos, Perdoes</t>
-        </is>
-      </c>
+      <c r="F12" s="5" t="inlineStr"/>
       <c r="G12" s="5" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="G13" s="6" t="inlineStr">
         <is>
-          <t>Horários ocupados: 9/66</t>
+          <t>Horários ocupados: 14/66</t>
         </is>
       </c>
     </row>
@@ -1473,20 +1317,32 @@
           <t>08:00</t>
         </is>
       </c>
-      <c r="B2" s="5" t="inlineStr"/>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>68 : 52 anos, Perdoes | 87 : 23 anos, Itajuba</t>
+        </is>
+      </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>57 : 52 anos, Bambui</t>
+          <t>6 : 23 anos, Lavras | 57 : 52 anos, Bambui | 61 : 22 anos, Lavras</t>
         </is>
       </c>
       <c r="D2" s="5" t="inlineStr"/>
-      <c r="E2" s="5" t="inlineStr"/>
+      <c r="E2" s="4" t="inlineStr">
+        <is>
+          <t>21 : 62 anos, Bambui | 65 : 50 anos, Lavras</t>
+        </is>
+      </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>16 : 20 anos, Bambui</t>
-        </is>
-      </c>
-      <c r="G2" s="5" t="inlineStr"/>
+          <t>99 : 25 anos, Lavras</t>
+        </is>
+      </c>
+      <c r="G2" s="3" t="inlineStr">
+        <is>
+          <t>52 : 22 anos, Perdoes | 62 : 50 anos, Perdoes | 79 : 17 anos, Perdoes</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="40" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
@@ -1494,16 +1350,32 @@
           <t>09:00</t>
         </is>
       </c>
-      <c r="B3" s="5" t="inlineStr"/>
-      <c r="C3" s="5" t="inlineStr"/>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>12 : 27 anos, Uberaba | 41 : 21 anos, Ijaci | 58 : 22 anos, Lavras | 70 : 21 anos, Ijaci | 82 : 21 anos, Vicosa</t>
+        </is>
+      </c>
+      <c r="C3" s="4" t="inlineStr">
+        <is>
+          <t>22 : 60 anos, Bambui</t>
+        </is>
+      </c>
       <c r="D3" s="3" t="inlineStr">
         <is>
           <t>7 : 24 anos, Bambui</t>
         </is>
       </c>
-      <c r="E3" s="5" t="inlineStr"/>
+      <c r="E3" s="3" t="inlineStr">
+        <is>
+          <t>53 : 21 anos, Ilheus</t>
+        </is>
+      </c>
       <c r="F3" s="5" t="inlineStr"/>
-      <c r="G3" s="5" t="inlineStr"/>
+      <c r="G3" s="3" t="inlineStr">
+        <is>
+          <t>60 : 21 anos, Lavras</t>
+        </is>
+      </c>
     </row>
     <row r="4" ht="40" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
@@ -1511,15 +1383,23 @@
           <t>10:00</t>
         </is>
       </c>
-      <c r="B4" s="3" t="inlineStr">
+      <c r="B4" s="4" t="inlineStr">
+        <is>
+          <t>26 : 20 anos, Lavras</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="inlineStr">
         <is>
           <t>97 : 54 anos, Bambui</t>
         </is>
       </c>
-      <c r="C4" s="5" t="inlineStr"/>
       <c r="D4" s="5" t="inlineStr"/>
       <c r="E4" s="5" t="inlineStr"/>
-      <c r="F4" s="5" t="inlineStr"/>
+      <c r="F4" s="3" t="inlineStr">
+        <is>
+          <t>51 : 26 anos, Macuco de Minas</t>
+        </is>
+      </c>
       <c r="G4" s="5" t="inlineStr"/>
     </row>
     <row r="5" ht="40" customHeight="1">
@@ -1528,12 +1408,32 @@
           <t>11:00</t>
         </is>
       </c>
-      <c r="B5" s="5" t="inlineStr"/>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>37 : 19 anos, Lavras</t>
+        </is>
+      </c>
       <c r="C5" s="5" t="inlineStr"/>
-      <c r="D5" s="5" t="inlineStr"/>
-      <c r="E5" s="5" t="inlineStr"/>
-      <c r="F5" s="5" t="inlineStr"/>
-      <c r="G5" s="5" t="inlineStr"/>
+      <c r="D5" s="3" t="inlineStr">
+        <is>
+          <t>2 : 21 anos, Lavras | 17 : 19 anos, Sao Paulo | 39 : 23 anos, Sao Joao Del Rei | 63 : 20 anos, Perdoes | 95 : 24 anos, Itajuba</t>
+        </is>
+      </c>
+      <c r="E5" s="4" t="inlineStr">
+        <is>
+          <t>36 : 71 anos, Guarapari</t>
+        </is>
+      </c>
+      <c r="F5" s="4" t="inlineStr">
+        <is>
+          <t>69 : 32 anos, Lavras</t>
+        </is>
+      </c>
+      <c r="G5" s="3" t="inlineStr">
+        <is>
+          <t>86 : 22 anos, Oliveira</t>
+        </is>
+      </c>
     </row>
     <row r="6" ht="40" customHeight="1">
       <c r="A6" s="2" t="inlineStr">
@@ -1544,7 +1444,11 @@
       <c r="B6" s="5" t="inlineStr"/>
       <c r="C6" s="5" t="inlineStr"/>
       <c r="D6" s="5" t="inlineStr"/>
-      <c r="E6" s="5" t="inlineStr"/>
+      <c r="E6" s="3" t="inlineStr">
+        <is>
+          <t>14 : 21 anos, Japaraiba</t>
+        </is>
+      </c>
       <c r="F6" s="5" t="inlineStr"/>
       <c r="G6" s="5" t="inlineStr"/>
     </row>
@@ -1554,16 +1458,24 @@
           <t>13:00</t>
         </is>
       </c>
-      <c r="B7" s="3" t="inlineStr">
+      <c r="B7" s="5" t="inlineStr"/>
+      <c r="C7" s="5" t="inlineStr"/>
+      <c r="D7" s="3" t="inlineStr">
+        <is>
+          <t>45 : 22 anos, Campo Belo</t>
+        </is>
+      </c>
+      <c r="E7" s="3" t="inlineStr">
         <is>
           <t>20 : 52 anos, Bambui</t>
         </is>
       </c>
-      <c r="C7" s="5" t="inlineStr"/>
-      <c r="D7" s="5" t="inlineStr"/>
-      <c r="E7" s="5" t="inlineStr"/>
       <c r="F7" s="5" t="inlineStr"/>
-      <c r="G7" s="5" t="inlineStr"/>
+      <c r="G7" s="3" t="inlineStr">
+        <is>
+          <t>40 : 23 anos, Perdoes | 75 : 31 anos, Lavras</t>
+        </is>
+      </c>
     </row>
     <row r="8" ht="40" customHeight="1">
       <c r="A8" s="2" t="inlineStr">
@@ -1571,11 +1483,19 @@
           <t>14:00</t>
         </is>
       </c>
-      <c r="B8" s="5" t="inlineStr"/>
-      <c r="C8" s="5" t="inlineStr"/>
+      <c r="B8" s="3" t="inlineStr">
+        <is>
+          <t>25 : 21 anos, Bambui</t>
+        </is>
+      </c>
+      <c r="C8" s="3" t="inlineStr">
+        <is>
+          <t>44 : 21 anos, Varginha</t>
+        </is>
+      </c>
       <c r="D8" s="3" t="inlineStr">
         <is>
-          <t>27 : 49 anos, Bambui | 59 : 21 anos, Bambui | 67 : 20 anos, Bambui</t>
+          <t>27 : 49 anos, Bambui</t>
         </is>
       </c>
       <c r="E8" s="3" t="inlineStr">
@@ -1584,7 +1504,11 @@
         </is>
       </c>
       <c r="F8" s="5" t="inlineStr"/>
-      <c r="G8" s="5" t="inlineStr"/>
+      <c r="G8" s="3" t="inlineStr">
+        <is>
+          <t>8 : 21 anos, Osasco</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="40" customHeight="1">
       <c r="A9" s="2" t="inlineStr">
@@ -1594,22 +1518,34 @@
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>38 : 19 anos, Bambui</t>
-        </is>
-      </c>
-      <c r="C9" s="5" t="inlineStr"/>
+          <t>38 : 19 anos, Bambui | 66 : 15 anos, Lavras</t>
+        </is>
+      </c>
+      <c r="C9" s="3" t="inlineStr">
+        <is>
+          <t>16 : 20 anos, Bambui | 64 : 21 anos, Oliveira | 83 : 20 anos, Lagoa da Prata</t>
+        </is>
+      </c>
       <c r="D9" s="3" t="inlineStr">
         <is>
-          <t>25 : 21 anos, Bambui | 31 : 35 anos, Bambui</t>
+          <t>31 : 35 anos, Bambui | 48 : 22 anos, Varginha</t>
         </is>
       </c>
       <c r="E9" s="3" t="inlineStr">
         <is>
-          <t>18 : 49 anos, Bambui</t>
-        </is>
-      </c>
-      <c r="F9" s="5" t="inlineStr"/>
-      <c r="G9" s="5" t="inlineStr"/>
+          <t>9 : 29 anos, Araraquara | 18 : 49 anos, Bambui | 80 : 32 anos, Belo Horizonte | 89 : 22 anos, Divinopolis</t>
+        </is>
+      </c>
+      <c r="F9" s="3" t="inlineStr">
+        <is>
+          <t>100 : 23 anos, Ijaci</t>
+        </is>
+      </c>
+      <c r="G9" s="3" t="inlineStr">
+        <is>
+          <t>73 : 23 anos, Uba</t>
+        </is>
+      </c>
     </row>
     <row r="10" ht="40" customHeight="1">
       <c r="A10" s="2" t="inlineStr">
@@ -1617,16 +1553,20 @@
           <t>16:00</t>
         </is>
       </c>
-      <c r="B10" s="5" t="inlineStr"/>
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t>34 : 19 anos, Sorocaba | 50 : 19 anos, Perdoes</t>
+        </is>
+      </c>
       <c r="C10" s="5" t="inlineStr"/>
-      <c r="D10" s="4" t="inlineStr">
-        <is>
-          <t>21 : 62 anos, Bambui</t>
+      <c r="D10" s="3" t="inlineStr">
+        <is>
+          <t>1 : 20 anos, Bambui | 29 : 20 anos, Pocos de Caldas | 46 : 21 anos, Jundiai | 67 : 20 anos, Bambui</t>
         </is>
       </c>
       <c r="E10" s="3" t="inlineStr">
         <is>
-          <t>1 : 20 anos, Bambui | 42 : 21 anos, Bambui | 85 : 19 anos, Bambui</t>
+          <t>85 : 19 anos, Bambui</t>
         </is>
       </c>
       <c r="F10" s="3" t="inlineStr">
@@ -1634,7 +1574,11 @@
           <t>88 : 21 anos, Bambui</t>
         </is>
       </c>
-      <c r="G10" s="5" t="inlineStr"/>
+      <c r="G10" s="3" t="inlineStr">
+        <is>
+          <t>4 : 20 anos, Guarulhos | 54 : 29 anos, Lavras | 81 : 23 anos, Sao Paulo | 84 : 19 anos, Sorocaba</t>
+        </is>
+      </c>
     </row>
     <row r="11" ht="40" customHeight="1">
       <c r="A11" s="2" t="inlineStr">
@@ -1642,16 +1586,32 @@
           <t>17:00</t>
         </is>
       </c>
-      <c r="B11" s="5" t="inlineStr"/>
-      <c r="C11" s="5" t="inlineStr"/>
-      <c r="D11" s="4" t="inlineStr">
-        <is>
-          <t>22 : 60 anos, Bambui</t>
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t>98 : 22 anos, Perdoes</t>
+        </is>
+      </c>
+      <c r="C11" s="3" t="inlineStr">
+        <is>
+          <t>71 : 45 anos, Medeiros | 76 : 28 anos, Bom Sucesso</t>
+        </is>
+      </c>
+      <c r="D11" s="3" t="inlineStr">
+        <is>
+          <t>30 : 20 anos, Lagoa da Prata | 42 : 21 anos, Bambui | 59 : 21 anos, Bambui | 74 : 18 anos, Perdoes | 94 : 35 anos, Medeiros</t>
         </is>
       </c>
       <c r="E11" s="5" t="inlineStr"/>
-      <c r="F11" s="5" t="inlineStr"/>
-      <c r="G11" s="5" t="inlineStr"/>
+      <c r="F11" s="3" t="inlineStr">
+        <is>
+          <t>32 : 21 anos, Guarapari | 33 : 21 anos, Lavras | 43 : 24 anos, Perdoes | 55 : 16 anos, Perdoes | 78 : 21 anos, Espinosa</t>
+        </is>
+      </c>
+      <c r="G11" s="4" t="inlineStr">
+        <is>
+          <t>13 : 23 anos, Uberlandia | 91 : 37 anos, Lavras</t>
+        </is>
+      </c>
     </row>
     <row r="12" ht="40" customHeight="1">
       <c r="A12" s="2" t="inlineStr">
@@ -1659,17 +1619,41 @@
           <t>18:00</t>
         </is>
       </c>
-      <c r="B12" s="5" t="inlineStr"/>
-      <c r="C12" s="5" t="inlineStr"/>
-      <c r="D12" s="5" t="inlineStr"/>
-      <c r="E12" s="5" t="inlineStr"/>
-      <c r="F12" s="5" t="inlineStr"/>
-      <c r="G12" s="5" t="inlineStr"/>
+      <c r="B12" s="4" t="inlineStr">
+        <is>
+          <t>19 : 24 anos, Guarulhos</t>
+        </is>
+      </c>
+      <c r="C12" s="3" t="inlineStr">
+        <is>
+          <t>47 : 21 anos, Campo Belo | 90 : 21 anos, Lavras | 92 : 20 anos, Areado | 101 : 20 anos, Arcos</t>
+        </is>
+      </c>
+      <c r="D12" s="3" t="inlineStr">
+        <is>
+          <t>11 : 20 anos, Medeiros | 23 : 16 anos, Guarulhos | 28 : 21 anos, Oliveira | 49 : 23 anos, Perdoes</t>
+        </is>
+      </c>
+      <c r="E12" s="3" t="inlineStr">
+        <is>
+          <t>3 : 22 anos, Lavras | 35 : 42 anos, Colatina</t>
+        </is>
+      </c>
+      <c r="F12" s="3" t="inlineStr">
+        <is>
+          <t>15 : 20 anos, Lagoa da Prata | 24 : 19 anos, Arcos | 56 : 19 anos, Perdoes | 72 : 32 anos, Lavras</t>
+        </is>
+      </c>
+      <c r="G12" s="3" t="inlineStr">
+        <is>
+          <t>77 : 23 anos, Lavras | 96 : 21 anos, Lavras</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="G13" s="6" t="inlineStr">
         <is>
-          <t>Horários ocupados: 14/66</t>
+          <t>Horários ocupados: 49/66</t>
         </is>
       </c>
     </row>

</xml_diff>